<commit_message>
Replaced emails with ID
</commit_message>
<xml_diff>
--- a/Report/03-UX-Design/FirstSurvey/Survey1_Responses.xlsx
+++ b/Report/03-UX-Design/FirstSurvey/Survey1_Responses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellagryf-lowczowska/Documents/MSc/segp/project_repo/Group1Project/Report/03-UX-Design/FirstSurvey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA7E7EF9-23B9-9046-8798-AB1B20412EA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515926F5-E528-244F-B003-08413D98D131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>Email address</t>
-  </si>
-  <si>
     <t>Our current name for this application is 'Focus on Lock'. If you have any suggestions for a better name, please enter them below.</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>If you have any suggestions on layout and/or general aesthetic, please make them below.</t>
   </si>
   <si>
-    <t>gryflowczowska@gmail.com</t>
-  </si>
-  <si>
     <t>Focus in Lockdown</t>
   </si>
   <si>
@@ -82,9 +76,6 @@
     <t>not just sounds distracting, have news headlines, email / Whatsapp logo etc</t>
   </si>
   <si>
-    <t>sashasemple98@gmail.com</t>
-  </si>
-  <si>
     <t>Distractathon</t>
   </si>
   <si>
@@ -112,9 +103,6 @@
     <t xml:space="preserve">Could be cool to design it like a phone screen and then the notifications pop down from the top like an incoming message, or you get a phone call. </t>
   </si>
   <si>
-    <t>francesca.ryman1@gmail.com</t>
-  </si>
-  <si>
     <t>Lockdown focus?</t>
   </si>
   <si>
@@ -139,9 +127,6 @@
     <t>You could include a round where there are no distractions but have a fake loading screen with a timer for 2 minutes or so then see if they become worse at answering the questions after the loading as they have become distracted. You could ask them to answer a question at the end to see if they check their phone during that 2 minute loading time.</t>
   </si>
   <si>
-    <t>inihos95@gmail.com</t>
-  </si>
-  <si>
     <t>N/a</t>
   </si>
   <si>
@@ -157,9 +142,6 @@
     <t>Puzzles</t>
   </si>
   <si>
-    <t>griggs.hattie@gmail.com</t>
-  </si>
-  <si>
     <t>Advanced Sound (e.g. notification bells, incoming WhatsApp sound,  BBC News theme song).</t>
   </si>
   <si>
@@ -178,9 +160,6 @@
     <t>I like the aesthetic :)</t>
   </si>
   <si>
-    <t>jessica@coppins.org</t>
-  </si>
-  <si>
     <t xml:space="preserve">Advanced Sound: I often find my phone very distracting and impossible to work unless I put my phone on silent. </t>
   </si>
   <si>
@@ -193,9 +172,6 @@
     <t xml:space="preserve">The order of the game should change each time so it doesn't become predictable. </t>
   </si>
   <si>
-    <t>elerobertson@yahoo.com</t>
-  </si>
-  <si>
     <t>Advanced Animation (e.g. current news headlines spinning over the screen)., Advanced Sound (e.g. notification bells, incoming WhatsApp sound,  BBC News theme song)., Player specific demands. ie for those in family members, a children crying</t>
   </si>
   <si>
@@ -208,18 +184,12 @@
     <t>problem solving, or puzzles</t>
   </si>
   <si>
-    <t>georgegriff0205@gmail.com</t>
-  </si>
-  <si>
     <t>Hocus Pocus Focus, Focal point</t>
   </si>
   <si>
     <t>Advance animation</t>
   </si>
   <si>
-    <t>ssm.poon@hotmail.co.uk</t>
-  </si>
-  <si>
     <t>Locked into Distraction, LockDown with Distraction</t>
   </si>
   <si>
@@ -235,9 +205,6 @@
     <t>The prototype looked quite simple and plain. I think it needs to have more to make it more fun.</t>
   </si>
   <si>
-    <t>mitch.robertson@gmail.com</t>
-  </si>
-  <si>
     <t>Basic Animation (cartoons, fireworks etc)., Advanced Animation (e.g. current news headlines spinning over the screen)., Advanced Sound (e.g. notification bells, incoming WhatsApp sound,  BBC News theme song).</t>
   </si>
   <si>
@@ -253,9 +220,6 @@
     <t xml:space="preserve">Muted colours.. Easy to read.. </t>
   </si>
   <si>
-    <t>jr@jodunel.com</t>
-  </si>
-  <si>
     <t>Alarms</t>
   </si>
   <si>
@@ -265,9 +229,6 @@
     <t>During distractions banners across the bottom, log time to answer question with and without distractions to score with questions of a similar difficulty</t>
   </si>
   <si>
-    <t>Sarahpeel93@hotmail.co.uk</t>
-  </si>
-  <si>
     <t>linking to users facebook and displaying the users old statuses</t>
   </si>
   <si>
@@ -278,9 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">Should be something quite easy </t>
-  </si>
-  <si>
-    <t>kanetreadwell@gmail.com</t>
   </si>
   <si>
     <r>
@@ -325,9 +283,6 @@
     <t>Simple, minimalistic I think is stylish and fashionable atm</t>
   </si>
   <si>
-    <t>caris.fuller01@gmail.com</t>
-  </si>
-  <si>
     <t>Eye on the ball</t>
   </si>
   <si>
@@ -344,6 +299,9 @@
   </si>
   <si>
     <t>bright colours are normally quite distracting and bold text</t>
+  </si>
+  <si>
+    <t>Participant ID</t>
   </si>
 </sst>
 </file>
@@ -386,6 +344,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -412,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -431,7 +390,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,15 +816,15 @@
   </sheetPr>
   <dimension ref="A1:Q115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="136" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="5" width="52" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" customWidth="1"/>
@@ -873,35 +840,35 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -914,467 +881,466 @@
       <c r="A2" s="2">
         <v>44271.877915833335</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>44272.789001736106</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>44272.793137210647</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="9">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>44273.457916828702</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>44273.459345763884</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>45</v>
+      <c r="B6" s="9">
+        <v>5</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>44273.548889074074</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>52</v>
+      <c r="B7" s="9">
+        <v>6</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>44274.527892916667</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>57</v>
+      <c r="B8" s="9">
+        <v>7</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>44274.541179675929</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>62</v>
+      <c r="B9" s="9">
+        <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>44274.550149178242</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>65</v>
+      <c r="B10" s="9">
+        <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>44274.556578020834</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>71</v>
+      <c r="B11" s="9">
+        <v>10</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>44274.577470671298</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>77</v>
+      <c r="B12" s="9">
+        <v>11</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>44274.763735787041</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>81</v>
+      <c r="B13" s="9">
+        <v>12</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="56" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>44274.771815370375</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>86</v>
+      <c r="B14" s="9">
+        <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>44278.582257488422</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>93</v>
+      <c r="B15" s="9">
+        <v>14</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="13" x14ac:dyDescent="0.15">
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="B19" s="8"/>
+    <row r="19" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="24" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="25" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="26" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="27" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="28" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="3:3" ht="13" x14ac:dyDescent="0.15">

</xml_diff>